<commit_message>
V1.0.2 Testeado manejo de excepciones sistema con envio de correo y cambio de correo a usar variable de archivo config
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
   <si>
     <t>Name</t>
   </si>
@@ -192,6 +192,15 @@
   </si>
   <si>
     <t>Nombre de hoja de excel de entrada</t>
+  </si>
+  <si>
+    <t>CorreoExcepcion</t>
+  </si>
+  <si>
+    <t>mauricioquirogapalma@gmail.com</t>
+  </si>
+  <si>
+    <t>Correo al cual se envian las excepciones de aplicación</t>
   </si>
 </sst>
 </file>
@@ -580,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -702,7 +711,17 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1693,9 +1712,10 @@
   <phoneticPr fontId="2"/>
   <hyperlinks>
     <hyperlink ref="B8" r:id="rId1"/>
+    <hyperlink ref="B12" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>